<commit_message>
Finished development - Sprint 1
Completed:
Input of score and comment for 'Interesting'
Submission of feedback to database via PHP
Placeholder for 'create class' screen

Also updated documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Backlog 1.xlsx
+++ b/Documentation/Sprint Backlog 1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>NOT STARTED</t>
   </si>
@@ -62,32 +62,53 @@
     <t>Fri</t>
   </si>
   <si>
-    <t>Thur</t>
-  </si>
-  <si>
     <t>Spring 1: Total Hours remaining</t>
   </si>
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
   <si>
-    <t>[START DATE] - [END DATE]</t>
-  </si>
-  <si>
-    <t>1.4 - I want to be able to give feedback on how interesting the class was (and why)</t>
-  </si>
-  <si>
     <t>Create input method</t>
   </si>
   <si>
-    <t>2.3 - I want to give students the option to select why a particular area/factor was bad or good (from a list of predefined statements)</t>
+    <t>Conduct Sprint Review</t>
+  </si>
+  <si>
+    <t>Create PHP scripts</t>
+  </si>
+  <si>
+    <t>Create database</t>
+  </si>
+  <si>
+    <t>Link app to database via PHP</t>
+  </si>
+  <si>
+    <t>[19/01/2015] - [30/01/2015]</t>
+  </si>
+  <si>
+    <t>Discuss input methods with students</t>
+  </si>
+  <si>
+    <t>Discuss nature of comments with lecturers</t>
+  </si>
+  <si>
+    <t>Sprint 1: Ideal hours remaining:</t>
+  </si>
+  <si>
+    <t>Acceptance testing</t>
+  </si>
+  <si>
+    <t>1.1 - As a student I want to be able to give feedback on how interesting the class was (and why)</t>
+  </si>
+  <si>
+    <t>2.1 - As a lecturer I want to give students the option to select why a particular area/factor was bad or good (from a list of predefined statements)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +167,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -186,12 +216,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF63FF04"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -224,19 +254,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -329,60 +346,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -391,12 +508,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,6 +553,1021 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46754531978839431"/>
+          <c:y val="2.5334783201083771E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1: Ideal hours remaining:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Spring 1: Total Hours remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$26:$M$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-116456400"/>
+        <c:axId val="-116446608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-116456400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-116446608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-116446608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-116456400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>5442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>21770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,35 +1833,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" customWidth="1"/>
     <col min="2" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
+    <row r="1" spans="1:13" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="20"/>
     </row>
-    <row r="2" spans="1:12" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:13" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -745,9 +1875,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -760,9 +1890,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -775,10 +1905,10 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:13" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
@@ -790,9 +1920,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:13" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -804,25 +1934,26 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="26"/>
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="20"/>
     </row>
-    <row r="8" spans="1:12" ht="36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="36" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
@@ -856,11 +1987,14 @@
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>11</v>
+      <c r="L8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
@@ -872,11 +2006,12 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="9"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>15</v>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -888,18 +2023,19 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="10"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" s="8">
-        <v>10</v>
-      </c>
-      <c r="C11" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="23"/>
       <c r="D11" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -922,80 +2058,112 @@
       <c r="K11" s="8">
         <v>0</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="8">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="10"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="8">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="10"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="8">
-        <v>15</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="8">
-        <v>15</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0</v>
-      </c>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1004,50 +2172,386 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="10"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="M18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="8">
+        <v>5</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="8">
+        <v>5</v>
+      </c>
+      <c r="E20" s="8">
+        <v>4</v>
+      </c>
+      <c r="F20" s="8">
+        <v>2</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="8">
+        <v>5</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="8">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8">
+        <v>5</v>
+      </c>
+      <c r="F21" s="8">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0</v>
+      </c>
+      <c r="M21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="8">
+        <v>8</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="8">
+        <v>8</v>
+      </c>
+      <c r="E22" s="8">
+        <v>8</v>
+      </c>
+      <c r="F22" s="8">
+        <v>5</v>
+      </c>
+      <c r="G22" s="8">
+        <v>5</v>
+      </c>
+      <c r="H22" s="8">
+        <v>3</v>
+      </c>
+      <c r="I22" s="8">
+        <v>2</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
+      <c r="H23" s="8">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8">
+        <v>1</v>
+      </c>
+      <c r="J23" s="8">
+        <v>1</v>
+      </c>
+      <c r="K23" s="8">
+        <v>1</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+      <c r="M23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="25">
+        <v>27</v>
+      </c>
+      <c r="E25" s="25">
+        <v>21</v>
+      </c>
+      <c r="F25" s="25">
+        <v>18</v>
+      </c>
+      <c r="G25" s="25">
+        <v>15</v>
+      </c>
+      <c r="H25" s="25">
         <v>12</v>
       </c>
-      <c r="B16" s="12">
-        <f>SUM(B11:B14)</f>
-        <v>25</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12">
-        <f t="shared" ref="D16:L16" si="0">SUM(D11:D14)</f>
-        <v>25</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="I25" s="25">
+        <v>10</v>
+      </c>
+      <c r="J25" s="25">
+        <v>7</v>
+      </c>
+      <c r="K25" s="25">
+        <v>4</v>
+      </c>
+      <c r="L25" s="25">
+        <v>2</v>
+      </c>
+      <c r="M25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="12">
+        <f>SUM(D12,D17,D20,D21,D22,D23, D11, D16, D18, D13)</f>
+        <v>27</v>
+      </c>
+      <c r="E26" s="12">
+        <f t="shared" ref="E26:M26" si="0">SUM(E12,E17,E20,E21,E22,E23, E11, E16, E18, E13)</f>
+        <v>20</v>
+      </c>
+      <c r="F26" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F16" s="12">
+        <v>13</v>
+      </c>
+      <c r="G26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
+        <v>9</v>
+      </c>
+      <c r="H26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="12">
+        <v>6</v>
+      </c>
+      <c r="I26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="12">
+        <v>5</v>
+      </c>
+      <c r="J26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="12">
+        <v>3</v>
+      </c>
+      <c r="K26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="12">
+        <v>3</v>
+      </c>
+      <c r="L26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="12">
+        <v>1</v>
+      </c>
+      <c r="M26" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1059,5 +2563,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>